<commit_message>
Update: Threat Alert Report - 2026-01-15 10:02
</commit_message>
<xml_diff>
--- a/excel_routes/route_AJF_CAI_threats.xlsx
+++ b/excel_routes/route_AJF_CAI_threats.xlsx
@@ -1,121 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODERED\LAB\Artifacts\outputs\run_generated_110126_at_00.36\reports\excel_routes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB25CD6-9969-428F-A88B-E770B41D450C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="4524" windowWidth="15408" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="THREAT_ALERT" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="THREAT_ALERT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Air Cairo Flight</t>
-  </si>
-  <si>
-    <t>Market Threat Airline</t>
-  </si>
-  <si>
-    <t>OAL Fare Threat</t>
-  </si>
-  <si>
-    <t>Our Fare</t>
-  </si>
-  <si>
-    <t>Fare Dif</t>
-  </si>
-  <si>
-    <t>OAL Baggage</t>
-  </si>
-  <si>
-    <t>Our Baggage</t>
-  </si>
-  <si>
-    <t>Bag Allowance Dif</t>
-  </si>
-  <si>
-    <t>IMPACT</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>15-JAN-26</t>
-  </si>
-  <si>
-    <t>SM-322</t>
-  </si>
-  <si>
-    <t>Nile Air NP-120</t>
-  </si>
-  <si>
-    <t>LOW THREAT</t>
-  </si>
-  <si>
-    <t>SAR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3498DB"/>
-        <bgColor rgb="FF3498DB"/>
+        <fgColor rgb="003498DB"/>
+        <bgColor rgb="003498DB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD4EDDA"/>
-        <bgColor rgb="FFD4EDDA"/>
+        <fgColor rgb="00D4EDDA"/>
+        <bgColor rgb="00D4EDDA"/>
       </patternFill>
     </fill>
   </fills>
@@ -128,49 +62,99 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -458,94 +442,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="153.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="19" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Air Cairo Flight</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Market Threat Airline</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>OAL Fare Threat</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Our Fare</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fare Dif</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>OAL Baggage</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Our Baggage</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bag Allowance Dif</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>IMPACT</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>15-JAN-26</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>SM-322</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Nile Air NP-120</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>421</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>491</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>-70</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>421</v>
-      </c>
-      <c r="E2" s="2">
-        <v>458</v>
-      </c>
-      <c r="F2" s="2">
-        <v>-37</v>
-      </c>
-      <c r="G2" s="2">
-        <v>30</v>
-      </c>
-      <c r="H2" s="2">
-        <v>30</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-01-15 11:07
</commit_message>
<xml_diff>
--- a/excel_routes/route_AJF_CAI_threats.xlsx
+++ b/excel_routes/route_AJF_CAI_threats.xlsx
@@ -1,55 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODERED\LAB\Artifacts\outputs\run_generated_150126_at_08.22\reports\excel_routes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CA7CB9-BA90-4963-A277-955ED94A2E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2436" yWindow="4620" windowWidth="15408" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="THREAT_ALERT" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="THREAT_ALERT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Air Cairo Flight</t>
+  </si>
+  <si>
+    <t>Market Threat Airline</t>
+  </si>
+  <si>
+    <t>OAL Fare Threat</t>
+  </si>
+  <si>
+    <t>Our Fare</t>
+  </si>
+  <si>
+    <t>Fare Dif</t>
+  </si>
+  <si>
+    <t>OAL Baggage</t>
+  </si>
+  <si>
+    <t>Our Baggage</t>
+  </si>
+  <si>
+    <t>Bag Allowance Dif</t>
+  </si>
+  <si>
+    <t>IMPACT</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>15-JAN-26</t>
+  </si>
+  <si>
+    <t>SM-322</t>
+  </si>
+  <si>
+    <t>Nile Air NP-120</t>
+  </si>
+  <si>
+    <t>LOW THREAT</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="003498DB"/>
-        <bgColor rgb="003498DB"/>
+        <fgColor rgb="FF3498DB"/>
+        <bgColor rgb="FF3498DB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D4EDDA"/>
-        <bgColor rgb="00D4EDDA"/>
+        <fgColor rgb="FFD4EDDA"/>
+        <bgColor rgb="FFD4EDDA"/>
       </patternFill>
     </fill>
   </fills>
@@ -62,99 +128,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -442,132 +458,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="23" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="19" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="153.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Air Cairo Flight</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Market Threat Airline</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>OAL Fare Threat</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Our Fare</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Fare Dif</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>OAL Baggage</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Our Baggage</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Bag Allowance Dif</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>IMPACT</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Currency</t>
-        </is>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>15-JAN-26</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>SM-322</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Nile Air NP-120</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2">
         <v>421</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>491</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>-70</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="2">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>SAR</t>
-        </is>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>